<commit_message>
input taken from Excel sheet successfully
</commit_message>
<xml_diff>
--- a/GET 2021/ExcelFiles/inputSheet.xlsx
+++ b/GET 2021/ExcelFiles/inputSheet.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -122,6 +123,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -470,4 +475,18 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>